<commit_message>
confirm changes to namings
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28914"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VirJenDB\virjendb_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C18661E0-97F0-4042-99F0-5256449468FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD2D23E1-E27F-44F9-B6B4-B2A9F9717BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="2" xr2:uid="{D7962945-3ACF-49DB-B8FB-E785F5F91D27}"/>
   </bookViews>
@@ -422,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6889" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6907" uniqueCount="1118">
   <si>
     <t>VJDBv0.3</t>
   </si>
@@ -3565,9 +3565,6 @@
     <t>Biosample Accession</t>
   </si>
   <si>
-    <t>Sampling Date</t>
-  </si>
-  <si>
     <t>would be "Date" but to make distinction as there are multiple dates</t>
   </si>
   <si>
@@ -3592,7 +3589,7 @@
     <t>Should be curated into Baltimore classes; Is this a sequence attribute or sample or both? Represent in naming?</t>
   </si>
   <si>
-    <t>Completeness</t>
+    <t>Genome Completeness</t>
   </si>
   <si>
     <t>technically sample species or below</t>
@@ -3607,13 +3604,22 @@
     <t>Segment Name</t>
   </si>
   <si>
+    <t>NCBI Species</t>
+  </si>
+  <si>
     <t>NCBI Virus has only the virus species in this field, Taxonomy Descision</t>
   </si>
   <si>
-    <t>Plan about sources and vocabularies, RKI different from ENA, what about NCBI and environmental</t>
-  </si>
-  <si>
-    <t>This is defined different from the duplicate below. Meaning for submission Tool was to have a geographical level higher than countries (continents)</t>
+    <t>Plan about sources and vocabularies, RKI different from ENA, what about NCBI and environmental, leave it like that for now with NCBi input</t>
+  </si>
+  <si>
+    <t>ncbi_usa</t>
+  </si>
+  <si>
+    <t>NCBI USA</t>
+  </si>
+  <si>
+    <t>This is defined different from the duplicate below. Meaning for submission Tool was to have a geographical level higher than countries (continents). We keep it (mostly redundant), might be useful for later curation</t>
   </si>
   <si>
     <t>Analysis Accession</t>
@@ -3622,18 +3628,12 @@
     <t>might be duplicate with analysis description</t>
   </si>
   <si>
-    <t>Level</t>
+    <t>apply customization to vjdb , e.g. chromosome to genome or something</t>
   </si>
   <si>
     <t>Min Gap Length</t>
   </si>
   <si>
-    <t>Program</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>for submission this is always "clone or isolate"</t>
   </si>
   <si>
@@ -3655,12 +3655,27 @@
     <t>Longitude</t>
   </si>
   <si>
+    <t>Region unclear -&gt; Check again where it came from, recheck naming and vocabulary</t>
+  </si>
+  <si>
+    <t>as it is, for revision with data</t>
+  </si>
+  <si>
     <t>Experiment Accession</t>
   </si>
   <si>
     <t>Seperation of values good for submission, display should be in one, needs curation from ENA values, seperate Fields for submission?</t>
   </si>
   <si>
+    <t>These two private for submission, one field for public where it is combined and one for normalized values (also for filtering)</t>
+  </si>
+  <si>
+    <t>Lab Host Common Name</t>
+  </si>
+  <si>
+    <t>remove? Lab Passage 1 to 1 in public and rest in private for submission</t>
+  </si>
+  <si>
     <t>remove?</t>
   </si>
   <si>
@@ -3676,7 +3691,10 @@
     <t>Run Accession</t>
   </si>
   <si>
-    <t>Common Abbreviation</t>
+    <t>Serotype</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
   </si>
   <si>
     <t>No mapping, seems to  be NCBI Tax ID</t>
@@ -3694,6 +3712,9 @@
     <t>Publication DOI</t>
   </si>
   <si>
+    <t>needs curation before public</t>
+  </si>
+  <si>
     <t>Pubmed Accession</t>
   </si>
   <si>
@@ -3736,13 +3757,28 @@
     <t>This is not needed as in ENA as there it functions as memorable orientation for objects for the user, for us a ID for each object would be more suitable</t>
   </si>
   <si>
-    <t>What is that? -&gt; remove, not visible in ENA Webin Portal Submission</t>
+    <t>move all to additional metadata and remove here</t>
+  </si>
+  <si>
+    <t>What is that? -&gt; remove, not visible in ENA Webin Portal Submission, remove for now</t>
   </si>
   <si>
     <t>Study Description</t>
   </si>
   <si>
     <t>What is that? -&gt; remove, not visible in ENA Webin Portal Submision</t>
+  </si>
+  <si>
+    <t>virus_old_names</t>
+  </si>
+  <si>
+    <t>sequence_byte_range</t>
+  </si>
+  <si>
+    <t>sequence_path</t>
+  </si>
+  <si>
+    <t>insertion_date</t>
   </si>
 </sst>
 </file>
@@ -4038,7 +4074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -4192,12 +4228,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -17079,7 +17109,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765CDCC6-1CB9-4D09-8DD5-54FCC33BD049}">
   <dimension ref="A1:FP344"/>
   <sheetViews>
-    <sheetView topLeftCell="W20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AH49" sqref="AH49:AN52"/>
     </sheetView>
   </sheetViews>
@@ -37233,10 +37263,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6CF321-9E04-432C-B74A-785CBBCC1526}">
-  <dimension ref="A1:AW157"/>
+  <dimension ref="A1:AW161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL94" workbookViewId="0">
-      <selection activeCell="AW118" sqref="AW118"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="E160" sqref="E160:E161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.5703125" defaultRowHeight="15"/>
@@ -38473,10 +38503,10 @@
         <v>99</v>
       </c>
       <c r="AV9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AW9" s="4" t="s">
         <v>1046</v>
-      </c>
-      <c r="AW9" s="4" t="s">
-        <v>1047</v>
       </c>
     </row>
     <row r="10" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -38700,7 +38730,7 @@
         <v>132</v>
       </c>
       <c r="AW11" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="12" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -38871,7 +38901,7 @@
         <v>150</v>
       </c>
       <c r="AV13" s="41" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="14" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -38968,7 +38998,7 @@
         <v>158</v>
       </c>
       <c r="AV14" s="41" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="15" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -39061,7 +39091,7 @@
         <v>166</v>
       </c>
       <c r="AW15" s="40" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="16" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -39162,7 +39192,7 @@
         <v>173</v>
       </c>
       <c r="AW16" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="17" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -39259,7 +39289,7 @@
         <v>179</v>
       </c>
       <c r="AV17" s="4" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="18" spans="1:49" s="47" customFormat="1" ht="23.25" customHeight="1">
@@ -39651,7 +39681,7 @@
         <v>209</v>
       </c>
       <c r="AW21" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="22" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -39751,11 +39781,11 @@
       <c r="AU22" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="AV22" s="40" t="s">
-        <v>218</v>
+      <c r="AV22" s="38" t="s">
+        <v>216</v>
       </c>
       <c r="AW22" s="40" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="23" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -39852,7 +39882,7 @@
         <v>225</v>
       </c>
       <c r="AW23" s="40" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="24" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -39943,7 +39973,7 @@
         <v>232</v>
       </c>
       <c r="AV24" s="40" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="25" spans="1:49" s="47" customFormat="1" ht="23.25" customHeight="1">
@@ -40032,7 +40062,7 @@
         <v>239</v>
       </c>
       <c r="AW25" s="47" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="26" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -40193,7 +40223,7 @@
       <c r="AT27" s="48"/>
       <c r="AU27" s="48"/>
       <c r="AW27" s="51" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="28" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -40289,7 +40319,7 @@
         <v>262</v>
       </c>
       <c r="AW28" s="43" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="29" spans="1:49" s="51" customFormat="1" ht="23.25" customHeight="1">
@@ -40356,7 +40386,7 @@
       <c r="AT29" s="48"/>
       <c r="AU29" s="48"/>
       <c r="AW29" s="51" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="30" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -40449,7 +40479,7 @@
         <v>268</v>
       </c>
       <c r="AV30" s="43" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="31" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -40558,6 +40588,9 @@
       </c>
       <c r="AU31" s="38" t="s">
         <v>274</v>
+      </c>
+      <c r="AV31" s="40" t="s">
+        <v>1059</v>
       </c>
       <c r="AW31" s="40" t="s">
         <v>1060</v>
@@ -40869,95 +40902,95 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="35" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A35" s="54" t="s">
-        <v>307</v>
-      </c>
-      <c r="B35" s="54" t="s">
-        <v>308</v>
-      </c>
-      <c r="C35" s="54" t="s">
+    <row r="35" spans="1:49" s="47" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A35" s="45" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B35" s="45" t="s">
+        <v>1063</v>
+      </c>
+      <c r="C35" s="45" t="s">
         <v>309</v>
       </c>
-      <c r="D35" s="54" t="s">
+      <c r="D35" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="54"/>
-      <c r="K35" s="54"/>
-      <c r="L35" s="54"/>
-      <c r="M35" s="54" t="s">
+      <c r="E35" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="45"/>
+      <c r="K35" s="45"/>
+      <c r="L35" s="45"/>
+      <c r="M35" s="45" t="s">
         <v>310</v>
       </c>
-      <c r="N35" s="54"/>
-      <c r="O35" s="54"/>
-      <c r="P35" s="54"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55" t="s">
+      <c r="N35" s="45"/>
+      <c r="O35" s="45"/>
+      <c r="P35" s="45"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="S35" s="54" t="s">
+      <c r="S35" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="T35" s="54" t="s">
+      <c r="T35" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="U35" s="54"/>
-      <c r="V35" s="54" t="str">
+      <c r="U35" s="45"/>
+      <c r="V35" s="45" t="str">
         <f t="shared" si="2"/>
         <v>["NCBI Virus", "Sample", "Collection"]</v>
       </c>
-      <c r="W35" s="54" t="s">
+      <c r="W35" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="X35" s="54" t="s">
+      <c r="X35" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="Y35" s="54"/>
-      <c r="Z35" s="54" t="s">
+      <c r="Y35" s="45"/>
+      <c r="Z35" s="45" t="s">
         <v>310</v>
       </c>
-      <c r="AA35" s="54" t="s">
+      <c r="AA35" s="45" t="s">
         <v>311</v>
       </c>
-      <c r="AB35" s="54"/>
-      <c r="AC35" s="54" t="s">
+      <c r="AB35" s="45"/>
+      <c r="AC35" s="45" t="s">
         <v>312</v>
       </c>
-      <c r="AD35" s="54"/>
-      <c r="AE35" s="54"/>
-      <c r="AF35" s="54"/>
-      <c r="AG35" s="54"/>
-      <c r="AH35" s="54"/>
-      <c r="AI35" s="54"/>
-      <c r="AJ35" s="54"/>
-      <c r="AK35" s="54"/>
-      <c r="AL35" s="54"/>
-      <c r="AM35" s="54"/>
-      <c r="AN35" s="54"/>
-      <c r="AO35" s="54"/>
-      <c r="AP35" s="54"/>
-      <c r="AQ35" s="54"/>
-      <c r="AR35" s="56" t="s">
+      <c r="AD35" s="45"/>
+      <c r="AE35" s="45"/>
+      <c r="AF35" s="45"/>
+      <c r="AG35" s="45"/>
+      <c r="AH35" s="45"/>
+      <c r="AI35" s="45"/>
+      <c r="AJ35" s="45"/>
+      <c r="AK35" s="45"/>
+      <c r="AL35" s="45"/>
+      <c r="AM35" s="45"/>
+      <c r="AN35" s="45"/>
+      <c r="AO35" s="45"/>
+      <c r="AP35" s="45"/>
+      <c r="AQ35" s="45"/>
+      <c r="AR35" s="47" t="s">
         <v>129</v>
       </c>
-      <c r="AS35" s="56" t="s">
+      <c r="AS35" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="AT35" s="54" t="s">
+      <c r="AT35" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="AU35" s="54" t="s">
+      <c r="AU35" s="45" t="s">
         <v>308</v>
       </c>
-      <c r="AW35" s="56" t="s">
-        <v>1062</v>
+      <c r="AW35" s="47" t="s">
+        <v>1064</v>
       </c>
     </row>
     <row r="36" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -41046,7 +41079,7 @@
         <v>314</v>
       </c>
       <c r="AV36" s="43" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="37" spans="1:49" s="54" customFormat="1" ht="23.25" customHeight="1">
@@ -41071,10 +41104,10 @@
       <c r="H37" s="54" t="s">
         <v>321</v>
       </c>
-      <c r="Q37" s="65" t="s">
+      <c r="Q37" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="R37" s="65" t="s">
+      <c r="R37" s="63" t="s">
         <v>72</v>
       </c>
       <c r="S37" s="54" t="s">
@@ -41112,7 +41145,7 @@
         <v>319</v>
       </c>
       <c r="AW37" s="54" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="38" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -41207,7 +41240,10 @@
         <v>323</v>
       </c>
       <c r="AV38" s="4" t="s">
-        <v>1065</v>
+        <v>323</v>
+      </c>
+      <c r="AW38" s="4" t="s">
+        <v>1067</v>
       </c>
     </row>
     <row r="39" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -41300,7 +41336,7 @@
         <v>328</v>
       </c>
       <c r="AV39" s="4" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="40" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -41408,8 +41444,8 @@
       <c r="AU40" s="3" t="s">
         <v>332</v>
       </c>
-      <c r="AV40" s="4" t="s">
-        <v>1067</v>
+      <c r="AV40" s="3" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -41501,8 +41537,8 @@
       <c r="AU41" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="AV41" s="4" t="s">
-        <v>1068</v>
+      <c r="AV41" s="3" t="s">
+        <v>343</v>
       </c>
       <c r="AW41" s="4" t="s">
         <v>1069</v>
@@ -42026,86 +42062,89 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="47" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A47" s="54" t="s">
+    <row r="47" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A47" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="D47" s="54" t="s">
+      <c r="D47" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="54" t="s">
+      <c r="E47" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="F47" s="54" t="s">
+      <c r="F47" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="55"/>
-      <c r="R47" s="55" t="s">
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="35"/>
+      <c r="R47" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="S47" s="54" t="s">
+      <c r="S47" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="T47" s="54" t="s">
+      <c r="T47" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="U47" s="54"/>
-      <c r="V47" s="54" t="str">
+      <c r="U47" s="3"/>
+      <c r="V47" s="3" t="str">
         <f t="shared" si="2"/>
         <v>["Sample", "Collection"]</v>
       </c>
-      <c r="W47" s="54" t="s">
+      <c r="W47" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="X47" s="54" t="s">
+      <c r="X47" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="Y47" s="54"/>
-      <c r="Z47" s="54"/>
-      <c r="AA47" s="54"/>
-      <c r="AB47" s="54"/>
-      <c r="AC47" s="54"/>
-      <c r="AD47" s="54"/>
-      <c r="AE47" s="54"/>
-      <c r="AF47" s="54"/>
-      <c r="AG47" s="54"/>
-      <c r="AH47" s="54"/>
-      <c r="AI47" s="54"/>
-      <c r="AJ47" s="54"/>
-      <c r="AK47" s="54"/>
-      <c r="AL47" s="54"/>
-      <c r="AM47" s="54"/>
-      <c r="AN47" s="54"/>
-      <c r="AO47" s="54"/>
-      <c r="AP47" s="54"/>
-      <c r="AQ47" s="54"/>
-      <c r="AR47" s="56" t="s">
+      <c r="Y47" s="3"/>
+      <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="3"/>
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="3"/>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="3"/>
+      <c r="AG47" s="3"/>
+      <c r="AH47" s="3"/>
+      <c r="AI47" s="3"/>
+      <c r="AJ47" s="3"/>
+      <c r="AK47" s="3"/>
+      <c r="AL47" s="3"/>
+      <c r="AM47" s="3"/>
+      <c r="AN47" s="3"/>
+      <c r="AO47" s="3"/>
+      <c r="AP47" s="3"/>
+      <c r="AQ47" s="3"/>
+      <c r="AR47" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="AS47" s="56" t="s">
+      <c r="AS47" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="AT47" s="54" t="s">
+      <c r="AT47" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="AU47" s="54" t="s">
+      <c r="AU47" s="3" t="s">
         <v>308</v>
+      </c>
+      <c r="AW47" s="4" t="s">
+        <v>1076</v>
       </c>
     </row>
     <row r="48" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -42210,6 +42249,9 @@
       </c>
       <c r="AU48" s="38" t="s">
         <v>382</v>
+      </c>
+      <c r="AW48" s="40" t="s">
+        <v>1077</v>
       </c>
     </row>
     <row r="49" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -42496,7 +42538,7 @@
         <v>400</v>
       </c>
       <c r="AV51" s="43" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="52" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -42609,7 +42651,7 @@
         <v>404</v>
       </c>
       <c r="AW52" s="40" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="53" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -42697,6 +42739,9 @@
       <c r="AU53" s="38" t="s">
         <v>410</v>
       </c>
+      <c r="AW53" s="40" t="s">
+        <v>1080</v>
+      </c>
     </row>
     <row r="54" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
       <c r="A54" s="3" t="s">
@@ -43357,8 +43402,11 @@
       <c r="AU60" s="38" t="s">
         <v>439</v>
       </c>
+      <c r="AV60" s="40" t="s">
+        <v>1081</v>
+      </c>
       <c r="AW60" s="40" t="s">
-        <v>1078</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="61" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -43445,7 +43493,7 @@
         <v>445</v>
       </c>
       <c r="AW61" s="40" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="62" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -43538,7 +43586,7 @@
         <v>449</v>
       </c>
       <c r="AW62" s="40" t="s">
-        <v>1078</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="63" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -43653,7 +43701,7 @@
         <v>452</v>
       </c>
       <c r="AV63" s="40" t="s">
-        <v>1079</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="64" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -43750,7 +43798,7 @@
         <v>461</v>
       </c>
       <c r="AW64" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="65" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -44338,7 +44386,7 @@
         <v>493</v>
       </c>
       <c r="AV70" s="43" t="s">
-        <v>1080</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="71" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -44891,7 +44939,7 @@
         <v>523</v>
       </c>
       <c r="AV76" s="43" t="s">
-        <v>1081</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="77" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -44982,7 +45030,7 @@
         <v>527</v>
       </c>
       <c r="AV77" s="43" t="s">
-        <v>1082</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="78" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -45071,7 +45119,7 @@
         <v>531</v>
       </c>
       <c r="AW78" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="79" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -45188,7 +45236,7 @@
         <v>537</v>
       </c>
       <c r="AW79" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="80" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -45205,7 +45253,7 @@
         <v>51</v>
       </c>
       <c r="E80" s="38" t="s">
-        <v>145</v>
+        <v>727</v>
       </c>
       <c r="F80" s="38" t="s">
         <v>546</v>
@@ -45294,8 +45342,11 @@
       <c r="AU80" s="38" t="s">
         <v>547</v>
       </c>
+      <c r="AV80" s="40" t="s">
+        <v>1088</v>
+      </c>
       <c r="AW80" s="40" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="81" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -45382,7 +45433,7 @@
         <v>553</v>
       </c>
       <c r="AV81" s="40" t="s">
-        <v>1083</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="82" spans="1:49" s="40" customFormat="1" ht="23.25" customHeight="1">
@@ -45471,7 +45522,7 @@
         <v>557</v>
       </c>
       <c r="AW82" s="40" t="s">
-        <v>1084</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="83" spans="1:49" s="43" customFormat="1" ht="23.25" customHeight="1">
@@ -45572,7 +45623,7 @@
         <v>561</v>
       </c>
       <c r="AV83" s="43" t="s">
-        <v>1085</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="84" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -45754,7 +45805,7 @@
         <v>573</v>
       </c>
       <c r="AV85" s="4" t="s">
-        <v>1086</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="86" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -45939,7 +45990,7 @@
         <v>587</v>
       </c>
       <c r="AV87" s="4" t="s">
-        <v>1087</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="88" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -45956,7 +46007,7 @@
         <v>51</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>204</v>
+        <v>145</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>591</v>
@@ -46028,7 +46079,10 @@
         <v>592</v>
       </c>
       <c r="AV88" s="4" t="s">
-        <v>1088</v>
+        <v>1094</v>
+      </c>
+      <c r="AW88" s="4" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="89" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46045,7 +46099,7 @@
         <v>51</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>52</v>
+        <v>145</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>596</v>
@@ -46125,7 +46179,10 @@
         <v>597</v>
       </c>
       <c r="AV89" s="4" t="s">
-        <v>1089</v>
+        <v>1096</v>
+      </c>
+      <c r="AW89" s="4" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="90" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46220,7 +46277,7 @@
         <v>604</v>
       </c>
       <c r="AV90" s="4" t="s">
-        <v>1090</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="91" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46495,7 +46552,7 @@
         <v>622</v>
       </c>
       <c r="AV93" s="4" t="s">
-        <v>1091</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="94" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46598,7 +46655,7 @@
         <v>631</v>
       </c>
       <c r="AV94" s="4" t="s">
-        <v>1092</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="95" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46699,7 +46756,7 @@
         <v>638</v>
       </c>
       <c r="AV95" s="4" t="s">
-        <v>1093</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="96" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46800,7 +46857,7 @@
         <v>644</v>
       </c>
       <c r="AV96" s="4" t="s">
-        <v>1094</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="97" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -46903,7 +46960,7 @@
         <v>650</v>
       </c>
       <c r="AV97" s="4" t="s">
-        <v>1095</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="98" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47004,7 +47061,7 @@
         <v>656</v>
       </c>
       <c r="AV98" s="4" t="s">
-        <v>1096</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="99" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47107,7 +47164,7 @@
         <v>662</v>
       </c>
       <c r="AV99" s="4" t="s">
-        <v>1097</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="100" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47208,7 +47265,7 @@
         <v>669</v>
       </c>
       <c r="AV100" s="4" t="s">
-        <v>1098</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="101" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47311,7 +47368,7 @@
         <v>675</v>
       </c>
       <c r="AV101" s="4" t="s">
-        <v>1099</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="102" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47422,7 +47479,7 @@
         <v>682</v>
       </c>
       <c r="AV102" s="4" t="s">
-        <v>1100</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="103" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1">
@@ -47929,7 +47986,7 @@
         <v>714</v>
       </c>
       <c r="AV108" s="4" t="s">
-        <v>1101</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="109" spans="1:49" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
@@ -48034,257 +48091,260 @@
         <v>718</v>
       </c>
     </row>
-    <row r="110" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A110" s="57" t="s">
+    <row r="110" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A110" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="B110" s="58" t="s">
+      <c r="B110" s="56" t="s">
         <v>725</v>
       </c>
-      <c r="C110" s="57" t="s">
+      <c r="C110" s="55" t="s">
         <v>726</v>
       </c>
-      <c r="D110" s="57"/>
-      <c r="E110" s="57" t="s">
+      <c r="D110" s="55"/>
+      <c r="E110" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="O110" s="57" t="s">
+      <c r="O110" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="P110" s="57" t="s">
+      <c r="P110" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="Q110" s="59" t="s">
+      <c r="Q110" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="R110" s="59" t="s">
+      <c r="R110" s="57" t="s">
         <v>248</v>
       </c>
-      <c r="V110" s="57" t="str">
+      <c r="V110" s="55" t="str">
         <f t="shared" si="3"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Study", "VJDB Study"]</v>
       </c>
-      <c r="AJ110" s="57" t="s">
+      <c r="AJ110" s="55" t="s">
         <v>729</v>
       </c>
-      <c r="AK110" s="57"/>
-      <c r="AL110" s="57"/>
-      <c r="AM110" s="57" t="s">
+      <c r="AK110" s="55"/>
+      <c r="AL110" s="55"/>
+      <c r="AM110" s="55" t="s">
         <v>729</v>
       </c>
-      <c r="AN110" s="57"/>
-      <c r="AO110" s="57" t="s">
+      <c r="AN110" s="55"/>
+      <c r="AO110" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP110" s="57" t="s">
+      <c r="AP110" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ110" s="57" t="s">
+      <c r="AQ110" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR110" s="60" t="s">
+      <c r="AR110" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS110" s="60" t="s">
+      <c r="AS110" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT110" s="57" t="s">
+      <c r="AT110" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="AU110" s="58" t="s">
+      <c r="AU110" s="56" t="s">
         <v>725</v>
       </c>
-      <c r="AW110" s="58" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="111" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A111" s="57" t="s">
+      <c r="AW110" s="56" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A111" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="B111" s="58" t="s">
+      <c r="B111" s="56" t="s">
         <v>731</v>
       </c>
-      <c r="C111" s="57" t="s">
+      <c r="C111" s="55" t="s">
         <v>732</v>
       </c>
-      <c r="D111" s="57"/>
-      <c r="E111" s="57" t="s">
+      <c r="D111" s="55"/>
+      <c r="E111" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="O111" s="57" t="s">
+      <c r="O111" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="P111" s="57" t="s">
+      <c r="P111" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="Q111" s="59" t="s">
+      <c r="Q111" s="57" t="s">
         <v>626</v>
       </c>
-      <c r="R111" s="59" t="s">
+      <c r="R111" s="57" t="s">
         <v>627</v>
       </c>
-      <c r="V111" s="57" t="str">
+      <c r="V111" s="55" t="str">
         <f t="shared" si="3"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Experiment", "VJDB Experiment"]</v>
       </c>
-      <c r="AJ111" s="57" t="s">
+      <c r="AJ111" s="55" t="s">
         <v>733</v>
       </c>
-      <c r="AK111" s="57"/>
-      <c r="AL111" s="57"/>
-      <c r="AM111" s="57" t="s">
+      <c r="AK111" s="55"/>
+      <c r="AL111" s="55"/>
+      <c r="AM111" s="55" t="s">
         <v>733</v>
       </c>
-      <c r="AN111" s="57"/>
-      <c r="AO111" s="57" t="s">
+      <c r="AN111" s="55"/>
+      <c r="AO111" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP111" s="57" t="s">
+      <c r="AP111" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ111" s="57" t="s">
+      <c r="AQ111" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR111" s="60" t="s">
+      <c r="AR111" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS111" s="60" t="s">
+      <c r="AS111" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT111" s="57" t="s">
+      <c r="AT111" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="AU111" s="58" t="s">
+      <c r="AU111" s="56" t="s">
         <v>731</v>
       </c>
-      <c r="AW111" s="58" t="s">
-        <v>1102</v>
-      </c>
-    </row>
-    <row r="112" spans="1:49" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A112" s="3" t="s">
+      <c r="AW111" s="56" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A112" s="55" t="s">
         <v>734</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="56" t="s">
         <v>735</v>
       </c>
-      <c r="C112" s="3" t="s">
+      <c r="C112" s="55" t="s">
         <v>736</v>
       </c>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3" t="s">
+      <c r="D112" s="55"/>
+      <c r="E112" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="O112" s="3" t="s">
+      <c r="O112" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="P112" s="3" t="s">
+      <c r="P112" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="Q112" s="32" t="s">
+      <c r="Q112" s="57" t="s">
         <v>737</v>
       </c>
-      <c r="R112" s="32" t="s">
+      <c r="R112" s="57" t="s">
         <v>738</v>
       </c>
-      <c r="V112" s="3" t="str">
+      <c r="V112" s="55" t="str">
         <f t="shared" si="3"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Run", "VJDB Run"]</v>
       </c>
-      <c r="AJ112" s="3" t="s">
+      <c r="AJ112" s="55" t="s">
         <v>739</v>
       </c>
-      <c r="AK112" s="3"/>
-      <c r="AL112" s="3"/>
-      <c r="AM112" s="3" t="s">
+      <c r="AK112" s="55"/>
+      <c r="AL112" s="55"/>
+      <c r="AM112" s="55" t="s">
         <v>739</v>
       </c>
-      <c r="AN112" s="3"/>
-      <c r="AO112" s="3" t="s">
+      <c r="AN112" s="55"/>
+      <c r="AO112" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP112" s="3" t="s">
+      <c r="AP112" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ112" s="3" t="s">
+      <c r="AQ112" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR112" s="4" t="s">
+      <c r="AR112" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS112" s="4" t="s">
+      <c r="AS112" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT112" s="3" t="s">
+      <c r="AT112" s="55" t="s">
         <v>734</v>
       </c>
-      <c r="AU112" t="s">
+      <c r="AU112" s="56" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="113" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A113" s="57" t="s">
+      <c r="AW112" s="56" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A113" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="B113" s="58" t="s">
+      <c r="B113" s="56" t="s">
         <v>741</v>
       </c>
-      <c r="C113" s="57" t="s">
+      <c r="C113" s="55" t="s">
         <v>742</v>
       </c>
-      <c r="D113" s="57"/>
-      <c r="E113" s="57" t="s">
+      <c r="D113" s="55"/>
+      <c r="E113" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="O113" s="57" t="s">
+      <c r="O113" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="P113" s="57" t="s">
+      <c r="P113" s="55" t="s">
         <v>728</v>
       </c>
-      <c r="Q113" s="59" t="s">
+      <c r="Q113" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="R113" s="59" t="s">
+      <c r="R113" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="V113" s="57" t="str">
+      <c r="V113" s="55" t="str">
         <f t="shared" si="3"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Sample", "VJDB Sample"]</v>
       </c>
-      <c r="AJ113" s="57" t="s">
+      <c r="AJ113" s="55" t="s">
         <v>743</v>
       </c>
-      <c r="AK113" s="57"/>
-      <c r="AL113" s="57"/>
-      <c r="AM113" s="57" t="s">
+      <c r="AK113" s="55"/>
+      <c r="AL113" s="55"/>
+      <c r="AM113" s="55" t="s">
         <v>739</v>
       </c>
-      <c r="AN113" s="57"/>
-      <c r="AO113" s="57" t="s">
+      <c r="AN113" s="55"/>
+      <c r="AO113" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP113" s="57" t="s">
+      <c r="AP113" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ113" s="57" t="s">
+      <c r="AQ113" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR113" s="60" t="s">
+      <c r="AR113" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS113" s="60" t="s">
+      <c r="AS113" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT113" s="57" t="s">
+      <c r="AT113" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="AU113" s="58" t="s">
+      <c r="AU113" s="56" t="s">
         <v>741</v>
       </c>
-      <c r="AW113" s="58" t="s">
-        <v>1102</v>
+      <c r="AW113" s="56" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="114" spans="1:49" ht="23.25" customHeight="1" thickBot="1">
@@ -48507,68 +48567,68 @@
         <v>754</v>
       </c>
     </row>
-    <row r="118" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A118" s="57" t="s">
+    <row r="118" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A118" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="B118" s="58" t="s">
+      <c r="B118" s="56" t="s">
         <v>731</v>
       </c>
-      <c r="C118" s="57" t="s">
+      <c r="C118" s="55" t="s">
         <v>756</v>
       </c>
-      <c r="D118" s="57"/>
-      <c r="E118" s="57" t="s">
+      <c r="D118" s="55"/>
+      <c r="E118" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="O118" s="57" t="s">
+      <c r="O118" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="P118" s="57" t="s">
+      <c r="P118" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="Q118" s="59" t="s">
+      <c r="Q118" s="57" t="s">
         <v>737</v>
       </c>
-      <c r="R118" s="59" t="s">
+      <c r="R118" s="57" t="s">
         <v>738</v>
       </c>
-      <c r="V118" s="57" t="str">
+      <c r="V118" s="55" t="str">
         <f t="shared" si="3"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Run", "VJDB Run"]</v>
       </c>
-      <c r="AJ118" s="57" t="s">
+      <c r="AJ118" s="55" t="s">
         <v>756</v>
       </c>
-      <c r="AK118" s="57"/>
-      <c r="AL118" s="57"/>
-      <c r="AM118" s="57" t="s">
+      <c r="AK118" s="55"/>
+      <c r="AL118" s="55"/>
+      <c r="AM118" s="55" t="s">
         <v>756</v>
       </c>
-      <c r="AN118" s="57"/>
-      <c r="AO118" s="57" t="s">
+      <c r="AN118" s="55"/>
+      <c r="AO118" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP118" s="57" t="s">
+      <c r="AP118" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ118" s="57" t="s">
+      <c r="AQ118" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR118" s="60" t="s">
+      <c r="AR118" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS118" s="60" t="s">
+      <c r="AS118" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT118" s="57" t="s">
+      <c r="AT118" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="AU118" s="58" t="s">
+      <c r="AU118" s="56" t="s">
         <v>731</v>
       </c>
-      <c r="AW118" s="58" t="s">
-        <v>1102</v>
+      <c r="AW118" s="56" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="119" spans="1:49" ht="23.25" customHeight="1" thickBot="1">
@@ -49557,11 +49617,11 @@
         <v>806</v>
       </c>
     </row>
-    <row r="136" spans="1:49" s="63" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="136" spans="1:49" s="61" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="A136" s="38" t="s">
         <v>808</v>
       </c>
-      <c r="B136" s="63" t="s">
+      <c r="B136" s="61" t="s">
         <v>809</v>
       </c>
       <c r="C136" s="38" t="s">
@@ -49577,10 +49637,10 @@
       <c r="P136" s="38" t="s">
         <v>808</v>
       </c>
-      <c r="Q136" s="64" t="s">
+      <c r="Q136" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="R136" s="64" t="s">
+      <c r="R136" s="62" t="s">
         <v>248</v>
       </c>
       <c r="V136" s="38" t="str">
@@ -49614,11 +49674,11 @@
       <c r="AT136" s="38" t="s">
         <v>808</v>
       </c>
-      <c r="AU136" s="63" t="s">
+      <c r="AU136" s="61" t="s">
         <v>809</v>
       </c>
-      <c r="AW136" s="63" t="s">
-        <v>1103</v>
+      <c r="AW136" s="61" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="137" spans="1:49" ht="23.25" customHeight="1" thickBot="1">
@@ -49859,67 +49919,67 @@
         <v>821</v>
       </c>
     </row>
-    <row r="141" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A141" s="57" t="s">
+    <row r="141" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A141" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="B141" s="58" t="s">
+      <c r="B141" s="56" t="s">
         <v>741</v>
       </c>
-      <c r="C141" s="57" t="s">
+      <c r="C141" s="55" t="s">
         <v>824</v>
       </c>
-      <c r="D141" s="57"/>
-      <c r="E141" s="57" t="s">
+      <c r="D141" s="55"/>
+      <c r="E141" s="55" t="s">
         <v>145</v>
       </c>
-      <c r="O141" s="57" t="s">
+      <c r="O141" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="P141" s="57" t="s">
+      <c r="P141" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="Q141" s="59" t="s">
+      <c r="Q141" s="57" t="s">
         <v>626</v>
       </c>
-      <c r="R141" s="59" t="s">
+      <c r="R141" s="57" t="s">
         <v>627</v>
       </c>
-      <c r="V141" s="57" t="str">
+      <c r="V141" s="55" t="str">
         <f t="shared" si="4"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Experiment", "VJDB Experiment"]</v>
       </c>
-      <c r="AJ141" s="57" t="s">
+      <c r="AJ141" s="55" t="s">
         <v>824</v>
       </c>
-      <c r="AK141" s="57"/>
-      <c r="AL141" s="57"/>
-      <c r="AM141" s="57" t="s">
+      <c r="AK141" s="55"/>
+      <c r="AL141" s="55"/>
+      <c r="AM141" s="55" t="s">
         <v>824</v>
       </c>
-      <c r="AN141" s="57"/>
-      <c r="AO141" s="57" t="s">
+      <c r="AN141" s="55"/>
+      <c r="AO141" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP141" s="57" t="s">
+      <c r="AP141" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ141" s="57" t="s">
+      <c r="AQ141" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR141" s="60" t="s">
+      <c r="AR141" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS141" s="60" t="s">
+      <c r="AS141" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT141" s="57" t="s">
+      <c r="AT141" s="55" t="s">
         <v>740</v>
       </c>
-      <c r="AU141" s="58" t="s">
+      <c r="AU141" s="56" t="s">
         <v>741</v>
       </c>
-      <c r="AW141" s="58" t="s">
+      <c r="AW141" s="56" t="s">
         <v>380</v>
       </c>
     </row>
@@ -50100,11 +50160,11 @@
         <v>832</v>
       </c>
     </row>
-    <row r="145" spans="1:49" s="61" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="145" spans="1:49" s="59" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="A145" s="41" t="s">
         <v>834</v>
       </c>
-      <c r="B145" s="61" t="s">
+      <c r="B145" s="59" t="s">
         <v>835</v>
       </c>
       <c r="C145" s="41" t="s">
@@ -50120,10 +50180,10 @@
       <c r="P145" s="41" t="s">
         <v>834</v>
       </c>
-      <c r="Q145" s="62" t="s">
+      <c r="Q145" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="R145" s="62" t="s">
+      <c r="R145" s="60" t="s">
         <v>248</v>
       </c>
       <c r="V145" s="41" t="str">
@@ -50157,82 +50217,82 @@
       <c r="AT145" s="41" t="s">
         <v>834</v>
       </c>
-      <c r="AU145" s="61" t="s">
+      <c r="AU145" s="59" t="s">
         <v>835</v>
       </c>
-      <c r="AV145" s="61" t="s">
-        <v>1104</v>
-      </c>
-    </row>
-    <row r="146" spans="1:49" s="58" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A146" s="57" t="s">
+      <c r="AV145" s="59" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="146" spans="1:49" s="56" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+      <c r="A146" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="B146" s="58" t="s">
+      <c r="B146" s="56" t="s">
         <v>725</v>
       </c>
-      <c r="C146" s="57" t="s">
+      <c r="C146" s="55" t="s">
         <v>838</v>
       </c>
-      <c r="D146" s="57"/>
-      <c r="E146" s="57" t="s">
+      <c r="D146" s="55"/>
+      <c r="E146" s="55" t="s">
         <v>727</v>
       </c>
-      <c r="O146" s="57" t="s">
+      <c r="O146" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="P146" s="57" t="s">
+      <c r="P146" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="Q146" s="59" t="s">
+      <c r="Q146" s="57" t="s">
         <v>626</v>
       </c>
-      <c r="R146" s="59" t="s">
+      <c r="R146" s="57" t="s">
         <v>627</v>
       </c>
-      <c r="V146" s="57" t="str">
+      <c r="V146" s="55" t="str">
         <f t="shared" si="4"/>
         <v>["ENA ERC32", "ENA ERC33", "ENA Experiment", "VJDB Experiment"]</v>
       </c>
-      <c r="AJ146" s="57" t="s">
+      <c r="AJ146" s="55" t="s">
         <v>838</v>
       </c>
-      <c r="AK146" s="57"/>
-      <c r="AL146" s="57"/>
-      <c r="AM146" s="57" t="s">
+      <c r="AK146" s="55"/>
+      <c r="AL146" s="55"/>
+      <c r="AM146" s="55" t="s">
         <v>838</v>
       </c>
-      <c r="AN146" s="57"/>
-      <c r="AO146" s="57" t="s">
+      <c r="AN146" s="55"/>
+      <c r="AO146" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="AP146" s="57" t="s">
+      <c r="AP146" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AQ146" s="57" t="s">
+      <c r="AQ146" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="AR146" s="60" t="s">
+      <c r="AR146" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="AS146" s="60" t="s">
+      <c r="AS146" s="58" t="s">
         <v>114</v>
       </c>
-      <c r="AT146" s="57" t="s">
+      <c r="AT146" s="55" t="s">
         <v>724</v>
       </c>
-      <c r="AU146" s="58" t="s">
+      <c r="AU146" s="56" t="s">
         <v>725</v>
       </c>
-      <c r="AW146" s="58" t="s">
+      <c r="AW146" s="56" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="147" spans="1:49" s="63" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
+    <row r="147" spans="1:49" s="61" customFormat="1" ht="23.25" customHeight="1" thickBot="1">
       <c r="A147" s="38" t="s">
         <v>839</v>
       </c>
-      <c r="B147" s="63" t="s">
+      <c r="B147" s="61" t="s">
         <v>840</v>
       </c>
       <c r="C147" s="38" t="s">
@@ -50248,10 +50308,10 @@
       <c r="P147" s="38" t="s">
         <v>839</v>
       </c>
-      <c r="Q147" s="64" t="s">
+      <c r="Q147" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="R147" s="64" t="s">
+      <c r="R147" s="62" t="s">
         <v>248</v>
       </c>
       <c r="V147" s="38" t="str">
@@ -50285,11 +50345,11 @@
       <c r="AT147" s="38" t="s">
         <v>839</v>
       </c>
-      <c r="AU147" s="63" t="s">
+      <c r="AU147" s="61" t="s">
         <v>840</v>
       </c>
-      <c r="AW147" s="63" t="s">
-        <v>1105</v>
+      <c r="AW147" s="61" t="s">
+        <v>1113</v>
       </c>
     </row>
     <row r="148" spans="1:49" ht="23.25" customHeight="1" thickBot="1">
@@ -50876,6 +50936,38 @@
       </c>
       <c r="AU157" t="s">
         <v>873</v>
+      </c>
+    </row>
+    <row r="158" spans="1:49">
+      <c r="A158" t="s">
+        <v>1114</v>
+      </c>
+      <c r="E158" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="159" spans="1:49">
+      <c r="A159" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E159" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="160" spans="1:49">
+      <c r="A160" t="s">
+        <v>1116</v>
+      </c>
+      <c r="E160" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E161" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>